<commit_message>
Initial 3.0.0 commit with RMI files (some additional updates still needed)
</commit_message>
<xml_diff>
--- a/InputData/add-outputs/SCoC/Social Cost of Carbon.xlsx
+++ b/InputData/add-outputs/SCoC/Social Cost of Carbon.xlsx
@@ -1,22 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Meghan\Dropbox (Energy Innovation)\EPS Versions\eps-1.5.0-us-wipI\InputData\add-outputs\SCoC\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="21080" windowHeight="11820"/>
+    <workbookView xWindow="480" yWindow="60" windowWidth="21075" windowHeight="11820"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
     <sheet name="SourceData" sheetId="2" r:id="rId2"/>
     <sheet name="SCoC" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="22">
   <si>
     <t>Source:</t>
   </si>
@@ -45,9 +50,6 @@
     <t>Source Data in 2007 dollars/metric ton CO2</t>
   </si>
   <si>
-    <t>Social Cost of Carbon ($)</t>
-  </si>
-  <si>
     <t>Data in 2012 dollars/gram CO2</t>
   </si>
   <si>
@@ -55,9 +57,6 @@
   </si>
   <si>
     <t>Notes:</t>
-  </si>
-  <si>
-    <t>When considering the Social Cost of Carbon, the U.S. government typically uses the figures based on</t>
   </si>
   <si>
     <t>a 3% discount rate, so this is the rate we use in this model.</t>
@@ -72,19 +71,28 @@
     <t>See "cpi.xlsx" in the InputData folder for source information.</t>
   </si>
   <si>
+    <t>We adjust 2007 dollars to 2012 dollars using the following conversion factor:</t>
+  </si>
+  <si>
     <t>Page 17, Table A1</t>
   </si>
   <si>
     <t>https://www.whitehouse.gov/sites/default/files/omb/inforeg/scc-tsd-final-july-2015.pdf</t>
   </si>
   <si>
-    <t>We adjust 2007 dollars to 2017 dollars using the following conversion factor:</t>
+    <t>Social Cost of Carbon ($/g CO2e)</t>
+  </si>
+  <si>
+    <t>When considering the Social Cost of Carbon, meant to capture the long-term economic damage caused by one</t>
+  </si>
+  <si>
+    <t>ton of carbon dioxide emitted, the U.S. government typically uses the figures based on</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.0%"/>
     <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0"/>
@@ -266,6 +274,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -313,7 +324,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -348,7 +359,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -557,20 +568,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B17"/>
+  <dimension ref="A1:B18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="97.1796875" customWidth="1"/>
+    <col min="2" max="2" width="97.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -593,53 +604,57 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B6" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>14</v>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="13" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A16" s="13" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A15" s="13" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A16" s="13">
-        <f>1.109*1.068</f>
-        <v>1.184412</v>
-      </c>
-    </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A17" s="13" t="s">
-        <v>17</v>
+      <c r="A17" s="13">
+        <v>1.109</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A18" s="13" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>
@@ -652,17 +667,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K44"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.453125" customWidth="1"/>
-    <col min="7" max="7" width="13.81640625" customWidth="1"/>
+    <col min="1" max="1" width="13.42578125" customWidth="1"/>
+    <col min="7" max="7" width="13.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
         <v>8</v>
       </c>
@@ -671,14 +684,14 @@
       <c r="D1" s="9"/>
       <c r="E1" s="9"/>
       <c r="G1" s="10" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H1" s="11"/>
       <c r="I1" s="11"/>
       <c r="J1" s="11"/>
       <c r="K1" s="11"/>
     </row>
-    <row r="2" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>3</v>
       </c>
@@ -710,7 +723,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>5</v>
       </c>
@@ -742,7 +755,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="13">
         <v>2010</v>
       </c>
@@ -763,23 +776,23 @@
         <v>2010</v>
       </c>
       <c r="H4" s="12">
-        <f>B4*(About!$A$16)/10^6</f>
-        <v>1.184412E-5</v>
+        <f>B4*(About!$A$17)/10^6</f>
+        <v>1.1090000000000001E-5</v>
       </c>
       <c r="I4" s="12">
-        <f>C4*(About!$A$16)/10^6</f>
-        <v>3.6716771999999997E-5</v>
+        <f>C4*(About!$A$17)/10^6</f>
+        <v>3.4378999999999997E-5</v>
       </c>
       <c r="J4" s="12">
-        <f>D4*(About!$A$16)/10^6</f>
-        <v>5.9220600000000007E-5</v>
+        <f>D4*(About!$A$17)/10^6</f>
+        <v>5.5450000000000006E-5</v>
       </c>
       <c r="K4" s="12">
-        <f>E4*(About!$A$16)/10^6</f>
-        <v>1.01859432E-4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+        <f>E4*(About!$A$17)/10^6</f>
+        <v>9.5373999999999999E-5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="13">
         <v>2011</v>
       </c>
@@ -800,23 +813,23 @@
         <v>2011</v>
       </c>
       <c r="H5" s="12">
-        <f>B5*(About!$A$16)/10^6</f>
-        <v>1.3028532E-5</v>
+        <f>B5*(About!$A$17)/10^6</f>
+        <v>1.2199E-5</v>
       </c>
       <c r="I5" s="12">
-        <f>C5*(About!$A$16)/10^6</f>
-        <v>3.7901183999999998E-5</v>
+        <f>C5*(About!$A$17)/10^6</f>
+        <v>3.5487999999999996E-5</v>
       </c>
       <c r="J5" s="12">
-        <f>D5*(About!$A$16)/10^6</f>
-        <v>6.0405012000000001E-5</v>
+        <f>D5*(About!$A$17)/10^6</f>
+        <v>5.6558999999999998E-5</v>
       </c>
       <c r="K5" s="12">
-        <f>E5*(About!$A$16)/10^6</f>
-        <v>1.0659708E-4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+        <f>E5*(About!$A$17)/10^6</f>
+        <v>9.9810000000000008E-5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="13">
         <v>2012</v>
       </c>
@@ -837,23 +850,23 @@
         <v>2012</v>
       </c>
       <c r="H6" s="12">
-        <f>B6*(About!$A$16)/10^6</f>
-        <v>1.3028532E-5</v>
+        <f>B6*(About!$A$17)/10^6</f>
+        <v>1.2199E-5</v>
       </c>
       <c r="I6" s="12">
-        <f>C6*(About!$A$16)/10^6</f>
-        <v>3.9085596E-5</v>
+        <f>C6*(About!$A$17)/10^6</f>
+        <v>3.6597000000000002E-5</v>
       </c>
       <c r="J6" s="12">
-        <f>D6*(About!$A$16)/10^6</f>
-        <v>6.2773835999999997E-5</v>
+        <f>D6*(About!$A$17)/10^6</f>
+        <v>5.8777000000000003E-5</v>
       </c>
       <c r="K6" s="12">
-        <f>E6*(About!$A$16)/10^6</f>
-        <v>1.1015031600000001E-4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+        <f>E6*(About!$A$17)/10^6</f>
+        <v>1.03137E-4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="13">
         <v>2013</v>
       </c>
@@ -874,23 +887,23 @@
         <v>2013</v>
       </c>
       <c r="H7" s="12">
-        <f>B7*(About!$A$16)/10^6</f>
-        <v>1.3028532E-5</v>
+        <f>B7*(About!$A$17)/10^6</f>
+        <v>1.2199E-5</v>
       </c>
       <c r="I7" s="12">
-        <f>C7*(About!$A$16)/10^6</f>
-        <v>4.0270008000000001E-5</v>
+        <f>C7*(About!$A$17)/10^6</f>
+        <v>3.7706000000000001E-5</v>
       </c>
       <c r="J7" s="12">
-        <f>D7*(About!$A$16)/10^6</f>
-        <v>6.3958247999999998E-5</v>
+        <f>D7*(About!$A$17)/10^6</f>
+        <v>5.9885999999999995E-5</v>
       </c>
       <c r="K7" s="12">
-        <f>E7*(About!$A$16)/10^6</f>
-        <v>1.14887964E-4</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+        <f>E7*(About!$A$17)/10^6</f>
+        <v>1.0757299999999999E-4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="13">
         <v>2014</v>
       </c>
@@ -911,23 +924,23 @@
         <v>2014</v>
       </c>
       <c r="H8" s="12">
-        <f>B8*(About!$A$16)/10^6</f>
-        <v>1.3028532E-5</v>
+        <f>B8*(About!$A$17)/10^6</f>
+        <v>1.2199E-5</v>
       </c>
       <c r="I8" s="12">
-        <f>C8*(About!$A$16)/10^6</f>
-        <v>4.1454420000000002E-5</v>
+        <f>C8*(About!$A$17)/10^6</f>
+        <v>3.8815E-5</v>
       </c>
       <c r="J8" s="12">
-        <f>D8*(About!$A$16)/10^6</f>
-        <v>6.5142660000000013E-5</v>
+        <f>D8*(About!$A$17)/10^6</f>
+        <v>6.0994999999999995E-5</v>
       </c>
       <c r="K8" s="12">
-        <f>E8*(About!$A$16)/10^6</f>
-        <v>1.19625612E-4</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+        <f>E8*(About!$A$17)/10^6</f>
+        <v>1.12009E-4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="13">
         <v>2015</v>
       </c>
@@ -948,23 +961,23 @@
         <v>2015</v>
       </c>
       <c r="H9" s="12">
-        <f>B9*(About!$A$16)/10^6</f>
-        <v>1.3028532E-5</v>
+        <f>B9*(About!$A$17)/10^6</f>
+        <v>1.2199E-5</v>
       </c>
       <c r="I9" s="12">
-        <f>C9*(About!$A$16)/10^6</f>
-        <v>4.2638832000000003E-5</v>
+        <f>C9*(About!$A$17)/10^6</f>
+        <v>3.9923999999999999E-5</v>
       </c>
       <c r="J9" s="12">
-        <f>D9*(About!$A$16)/10^6</f>
-        <v>6.6327072000000001E-5</v>
+        <f>D9*(About!$A$17)/10^6</f>
+        <v>6.2104E-5</v>
       </c>
       <c r="K9" s="12">
-        <f>E9*(About!$A$16)/10^6</f>
-        <v>1.2436325999999999E-4</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+        <f>E9*(About!$A$17)/10^6</f>
+        <v>1.1644499999999999E-4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="13">
         <v>2016</v>
       </c>
@@ -985,23 +998,23 @@
         <v>2016</v>
       </c>
       <c r="H10" s="12">
-        <f>B10*(About!$A$16)/10^6</f>
-        <v>1.3028532E-5</v>
+        <f>B10*(About!$A$17)/10^6</f>
+        <v>1.2199E-5</v>
       </c>
       <c r="I10" s="12">
-        <f>C10*(About!$A$16)/10^6</f>
-        <v>4.5007655999999999E-5</v>
+        <f>C10*(About!$A$17)/10^6</f>
+        <v>4.2141999999999997E-5</v>
       </c>
       <c r="J10" s="12">
-        <f>D10*(About!$A$16)/10^6</f>
-        <v>6.7511484000000002E-5</v>
+        <f>D10*(About!$A$17)/10^6</f>
+        <v>6.3213000000000006E-5</v>
       </c>
       <c r="K10" s="12">
-        <f>E10*(About!$A$16)/10^6</f>
-        <v>1.27916496E-4</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+        <f>E10*(About!$A$17)/10^6</f>
+        <v>1.1977199999999999E-4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="13">
         <v>2017</v>
       </c>
@@ -1022,23 +1035,23 @@
         <v>2017</v>
       </c>
       <c r="H11" s="12">
-        <f>B11*(About!$A$16)/10^6</f>
-        <v>1.3028532E-5</v>
+        <f>B11*(About!$A$17)/10^6</f>
+        <v>1.2199E-5</v>
       </c>
       <c r="I11" s="12">
-        <f>C11*(About!$A$16)/10^6</f>
-        <v>4.6192068E-5</v>
+        <f>C11*(About!$A$17)/10^6</f>
+        <v>4.3250999999999996E-5</v>
       </c>
       <c r="J11" s="12">
-        <f>D11*(About!$A$16)/10^6</f>
-        <v>6.9880308000000004E-5</v>
+        <f>D11*(About!$A$17)/10^6</f>
+        <v>6.5430999999999991E-5</v>
       </c>
       <c r="K11" s="12">
-        <f>E11*(About!$A$16)/10^6</f>
-        <v>1.32654144E-4</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+        <f>E11*(About!$A$17)/10^6</f>
+        <v>1.24208E-4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="13">
         <v>2018</v>
       </c>
@@ -1059,23 +1072,23 @@
         <v>2018</v>
       </c>
       <c r="H12" s="12">
-        <f>B12*(About!$A$16)/10^6</f>
-        <v>1.4212943999999999E-5</v>
+        <f>B12*(About!$A$17)/10^6</f>
+        <v>1.3308E-5</v>
       </c>
       <c r="I12" s="12">
-        <f>C12*(About!$A$16)/10^6</f>
-        <v>4.7376480000000001E-5</v>
+        <f>C12*(About!$A$17)/10^6</f>
+        <v>4.4360000000000002E-5</v>
       </c>
       <c r="J12" s="12">
-        <f>D12*(About!$A$16)/10^6</f>
-        <v>7.1064719999999992E-5</v>
+        <f>D12*(About!$A$17)/10^6</f>
+        <v>6.6539999999999997E-5</v>
       </c>
       <c r="K12" s="12">
-        <f>E12*(About!$A$16)/10^6</f>
-        <v>1.3739179200000001E-4</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+        <f>E12*(About!$A$17)/10^6</f>
+        <v>1.28644E-4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="13">
         <v>2019</v>
       </c>
@@ -1096,23 +1109,23 @@
         <v>2019</v>
       </c>
       <c r="H13" s="12">
-        <f>B13*(About!$A$16)/10^6</f>
-        <v>1.4212943999999999E-5</v>
+        <f>B13*(About!$A$17)/10^6</f>
+        <v>1.3308E-5</v>
       </c>
       <c r="I13" s="12">
-        <f>C13*(About!$A$16)/10^6</f>
-        <v>4.8560892000000003E-5</v>
+        <f>C13*(About!$A$17)/10^6</f>
+        <v>4.5469000000000001E-5</v>
       </c>
       <c r="J13" s="12">
-        <f>D13*(About!$A$16)/10^6</f>
-        <v>7.2249132000000007E-5</v>
+        <f>D13*(About!$A$17)/10^6</f>
+        <v>6.7649000000000002E-5</v>
       </c>
       <c r="K13" s="12">
-        <f>E13*(About!$A$16)/10^6</f>
-        <v>1.4212943999999998E-4</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+        <f>E13*(About!$A$17)/10^6</f>
+        <v>1.3307999999999999E-4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="13">
         <v>2020</v>
       </c>
@@ -1133,23 +1146,23 @@
         <v>2020</v>
       </c>
       <c r="H14" s="12">
-        <f>B14*(About!$A$16)/10^6</f>
-        <v>1.4212943999999999E-5</v>
+        <f>B14*(About!$A$17)/10^6</f>
+        <v>1.3308E-5</v>
       </c>
       <c r="I14" s="12">
-        <f>C14*(About!$A$16)/10^6</f>
-        <v>4.9745304000000004E-5</v>
+        <f>C14*(About!$A$17)/10^6</f>
+        <v>4.6578E-5</v>
       </c>
       <c r="J14" s="12">
-        <f>D14*(About!$A$16)/10^6</f>
-        <v>7.3433543999999994E-5</v>
+        <f>D14*(About!$A$17)/10^6</f>
+        <v>6.8757999999999995E-5</v>
       </c>
       <c r="K14" s="12">
-        <f>E14*(About!$A$16)/10^6</f>
-        <v>1.4568267600000001E-4</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+        <f>E14*(About!$A$17)/10^6</f>
+        <v>1.3640700000000001E-4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="13">
         <v>2021</v>
       </c>
@@ -1170,23 +1183,23 @@
         <v>2021</v>
       </c>
       <c r="H15" s="12">
-        <f>B15*(About!$A$16)/10^6</f>
-        <v>1.4212943999999999E-5</v>
+        <f>B15*(About!$A$17)/10^6</f>
+        <v>1.3308E-5</v>
       </c>
       <c r="I15" s="12">
-        <f>C15*(About!$A$16)/10^6</f>
-        <v>4.9745304000000004E-5</v>
+        <f>C15*(About!$A$17)/10^6</f>
+        <v>4.6578E-5</v>
       </c>
       <c r="J15" s="12">
-        <f>D15*(About!$A$16)/10^6</f>
-        <v>7.4617956000000009E-5</v>
+        <f>D15*(About!$A$17)/10^6</f>
+        <v>6.9867E-5</v>
       </c>
       <c r="K15" s="12">
-        <f>E15*(About!$A$16)/10^6</f>
-        <v>1.4923591200000002E-4</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+        <f>E15*(About!$A$17)/10^6</f>
+        <v>1.39734E-4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="13">
         <v>2022</v>
       </c>
@@ -1207,23 +1220,23 @@
         <v>2022</v>
       </c>
       <c r="H16" s="12">
-        <f>B16*(About!$A$16)/10^6</f>
-        <v>1.5397355999999999E-5</v>
+        <f>B16*(About!$A$17)/10^6</f>
+        <v>1.4416999999999999E-5</v>
       </c>
       <c r="I16" s="12">
-        <f>C16*(About!$A$16)/10^6</f>
-        <v>5.0929715999999998E-5</v>
+        <f>C16*(About!$A$17)/10^6</f>
+        <v>4.7686999999999999E-5</v>
       </c>
       <c r="J16" s="12">
-        <f>D16*(About!$A$16)/10^6</f>
-        <v>7.5802367999999997E-5</v>
+        <f>D16*(About!$A$17)/10^6</f>
+        <v>7.0975999999999993E-5</v>
       </c>
       <c r="K16" s="12">
-        <f>E16*(About!$A$16)/10^6</f>
-        <v>1.5278914800000002E-4</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+        <f>E16*(About!$A$17)/10^6</f>
+        <v>1.4306100000000002E-4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="13">
         <v>2023</v>
       </c>
@@ -1244,23 +1257,23 @@
         <v>2023</v>
       </c>
       <c r="H17" s="12">
-        <f>B17*(About!$A$16)/10^6</f>
-        <v>1.5397355999999999E-5</v>
+        <f>B17*(About!$A$17)/10^6</f>
+        <v>1.4416999999999999E-5</v>
       </c>
       <c r="I17" s="12">
-        <f>C17*(About!$A$16)/10^6</f>
-        <v>5.2114128E-5</v>
+        <f>C17*(About!$A$17)/10^6</f>
+        <v>4.8795999999999998E-5</v>
       </c>
       <c r="J17" s="12">
-        <f>D17*(About!$A$16)/10^6</f>
-        <v>7.6986779999999998E-5</v>
+        <f>D17*(About!$A$17)/10^6</f>
+        <v>7.2084999999999998E-5</v>
       </c>
       <c r="K17" s="12">
-        <f>E17*(About!$A$16)/10^6</f>
-        <v>1.56342384E-4</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+        <f>E17*(About!$A$17)/10^6</f>
+        <v>1.4638800000000001E-4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="13">
         <v>2024</v>
       </c>
@@ -1281,23 +1294,23 @@
         <v>2024</v>
       </c>
       <c r="H18" s="12">
-        <f>B18*(About!$A$16)/10^6</f>
-        <v>1.5397355999999999E-5</v>
+        <f>B18*(About!$A$17)/10^6</f>
+        <v>1.4416999999999999E-5</v>
       </c>
       <c r="I18" s="12">
-        <f>C18*(About!$A$16)/10^6</f>
-        <v>5.3298540000000001E-5</v>
+        <f>C18*(About!$A$17)/10^6</f>
+        <v>4.9905000000000004E-5</v>
       </c>
       <c r="J18" s="12">
-        <f>D18*(About!$A$16)/10^6</f>
-        <v>7.8171191999999999E-5</v>
+        <f>D18*(About!$A$17)/10^6</f>
+        <v>7.3194000000000004E-5</v>
       </c>
       <c r="K18" s="12">
-        <f>E18*(About!$A$16)/10^6</f>
-        <v>1.5989562E-4</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+        <f>E18*(About!$A$17)/10^6</f>
+        <v>1.49715E-4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="13">
         <v>2025</v>
       </c>
@@ -1318,23 +1331,23 @@
         <v>2025</v>
       </c>
       <c r="H19" s="12">
-        <f>B19*(About!$A$16)/10^6</f>
-        <v>1.6581768E-5</v>
+        <f>B19*(About!$A$17)/10^6</f>
+        <v>1.5526E-5</v>
       </c>
       <c r="I19" s="12">
-        <f>C19*(About!$A$16)/10^6</f>
-        <v>5.4482951999999995E-5</v>
+        <f>C19*(About!$A$17)/10^6</f>
+        <v>5.1013999999999996E-5</v>
       </c>
       <c r="J19" s="12">
-        <f>D19*(About!$A$16)/10^6</f>
-        <v>8.0540016000000002E-5</v>
+        <f>D19*(About!$A$17)/10^6</f>
+        <v>7.5412000000000002E-5</v>
       </c>
       <c r="K19" s="12">
-        <f>E19*(About!$A$16)/10^6</f>
-        <v>1.6344885600000001E-4</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+        <f>E19*(About!$A$17)/10^6</f>
+        <v>1.5304199999999999E-4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="13">
         <v>2026</v>
       </c>
@@ -1355,23 +1368,23 @@
         <v>2026</v>
       </c>
       <c r="H20" s="12">
-        <f>B20*(About!$A$16)/10^6</f>
-        <v>1.6581768E-5</v>
+        <f>B20*(About!$A$17)/10^6</f>
+        <v>1.5526E-5</v>
       </c>
       <c r="I20" s="12">
-        <f>C20*(About!$A$16)/10^6</f>
-        <v>5.5667363999999996E-5</v>
+        <f>C20*(About!$A$17)/10^6</f>
+        <v>5.2122999999999995E-5</v>
       </c>
       <c r="J20" s="12">
-        <f>D20*(About!$A$16)/10^6</f>
-        <v>8.1724428000000003E-5</v>
+        <f>D20*(About!$A$17)/10^6</f>
+        <v>7.6520999999999995E-5</v>
       </c>
       <c r="K20" s="12">
-        <f>E20*(About!$A$16)/10^6</f>
-        <v>1.6700209200000001E-4</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+        <f>E20*(About!$A$17)/10^6</f>
+        <v>1.5636900000000001E-4</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="13">
         <v>2027</v>
       </c>
@@ -1392,23 +1405,23 @@
         <v>2027</v>
       </c>
       <c r="H21" s="12">
-        <f>B21*(About!$A$16)/10^6</f>
-        <v>1.7766179999999998E-5</v>
+        <f>B21*(About!$A$17)/10^6</f>
+        <v>1.6634999999999999E-5</v>
       </c>
       <c r="I21" s="12">
-        <f>C21*(About!$A$16)/10^6</f>
-        <v>5.6851775999999998E-5</v>
+        <f>C21*(About!$A$17)/10^6</f>
+        <v>5.3232000000000001E-5</v>
       </c>
       <c r="J21" s="12">
-        <f>D21*(About!$A$16)/10^6</f>
-        <v>8.2908840000000004E-5</v>
+        <f>D21*(About!$A$17)/10^6</f>
+        <v>7.763E-5</v>
       </c>
       <c r="K21" s="12">
-        <f>E21*(About!$A$16)/10^6</f>
-        <v>1.6937091599999999E-4</v>
-      </c>
-    </row>
-    <row r="22" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+        <f>E21*(About!$A$17)/10^6</f>
+        <v>1.5858699999999999E-4</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="13">
         <v>2028</v>
       </c>
@@ -1429,23 +1442,23 @@
         <v>2028</v>
       </c>
       <c r="H22" s="12">
-        <f>B22*(About!$A$16)/10^6</f>
-        <v>1.7766179999999998E-5</v>
+        <f>B22*(About!$A$17)/10^6</f>
+        <v>1.6634999999999999E-5</v>
       </c>
       <c r="I22" s="12">
-        <f>C22*(About!$A$16)/10^6</f>
-        <v>5.8036188000000006E-5</v>
+        <f>C22*(About!$A$17)/10^6</f>
+        <v>5.4341E-5</v>
       </c>
       <c r="J22" s="12">
-        <f>D22*(About!$A$16)/10^6</f>
-        <v>8.4093252000000005E-5</v>
+        <f>D22*(About!$A$17)/10^6</f>
+        <v>7.8739000000000006E-5</v>
       </c>
       <c r="K22" s="12">
-        <f>E22*(About!$A$16)/10^6</f>
-        <v>1.7292415199999999E-4</v>
-      </c>
-    </row>
-    <row r="23" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+        <f>E22*(About!$A$17)/10^6</f>
+        <v>1.6191399999999998E-4</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="13">
         <v>2029</v>
       </c>
@@ -1466,23 +1479,23 @@
         <v>2029</v>
       </c>
       <c r="H23" s="12">
-        <f>B23*(About!$A$16)/10^6</f>
-        <v>1.7766179999999998E-5</v>
+        <f>B23*(About!$A$17)/10^6</f>
+        <v>1.6634999999999999E-5</v>
       </c>
       <c r="I23" s="12">
-        <f>C23*(About!$A$16)/10^6</f>
-        <v>5.8036188000000006E-5</v>
+        <f>C23*(About!$A$17)/10^6</f>
+        <v>5.4341E-5</v>
       </c>
       <c r="J23" s="12">
-        <f>D23*(About!$A$16)/10^6</f>
-        <v>8.5277664000000007E-5</v>
+        <f>D23*(About!$A$17)/10^6</f>
+        <v>7.9847999999999999E-5</v>
       </c>
       <c r="K23" s="12">
-        <f>E23*(About!$A$16)/10^6</f>
-        <v>1.7647738799999999E-4</v>
-      </c>
-    </row>
-    <row r="24" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+        <f>E23*(About!$A$17)/10^6</f>
+        <v>1.65241E-4</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" s="13">
         <v>2030</v>
       </c>
@@ -1503,23 +1516,23 @@
         <v>2030</v>
       </c>
       <c r="H24" s="12">
-        <f>B24*(About!$A$16)/10^6</f>
-        <v>1.8950591999999999E-5</v>
+        <f>B24*(About!$A$17)/10^6</f>
+        <v>1.7743999999999998E-5</v>
       </c>
       <c r="I24" s="12">
-        <f>C24*(About!$A$16)/10^6</f>
-        <v>5.9220600000000007E-5</v>
+        <f>C24*(About!$A$17)/10^6</f>
+        <v>5.5450000000000006E-5</v>
       </c>
       <c r="J24" s="12">
-        <f>D24*(About!$A$16)/10^6</f>
-        <v>8.6462075999999994E-5</v>
+        <f>D24*(About!$A$17)/10^6</f>
+        <v>8.0956999999999991E-5</v>
       </c>
       <c r="K24" s="12">
-        <f>E24*(About!$A$16)/10^6</f>
-        <v>1.80030624E-4</v>
-      </c>
-    </row>
-    <row r="25" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+        <f>E24*(About!$A$17)/10^6</f>
+        <v>1.6856799999999999E-4</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" s="13">
         <v>2031</v>
       </c>
@@ -1540,23 +1553,23 @@
         <v>2031</v>
       </c>
       <c r="H25" s="12">
-        <f>B25*(About!$A$16)/10^6</f>
-        <v>1.8950591999999999E-5</v>
+        <f>B25*(About!$A$17)/10^6</f>
+        <v>1.7743999999999998E-5</v>
       </c>
       <c r="I25" s="12">
-        <f>C25*(About!$A$16)/10^6</f>
-        <v>6.0405012000000001E-5</v>
+        <f>C25*(About!$A$17)/10^6</f>
+        <v>5.6558999999999998E-5</v>
       </c>
       <c r="J25" s="12">
-        <f>D25*(About!$A$16)/10^6</f>
-        <v>8.7646488000000009E-5</v>
+        <f>D25*(About!$A$17)/10^6</f>
+        <v>8.2065999999999997E-5</v>
       </c>
       <c r="K25" s="12">
-        <f>E25*(About!$A$16)/10^6</f>
-        <v>1.8358386000000003E-4</v>
-      </c>
-    </row>
-    <row r="26" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+        <f>E25*(About!$A$17)/10^6</f>
+        <v>1.7189500000000001E-4</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" s="13">
         <v>2032</v>
       </c>
@@ -1577,23 +1590,23 @@
         <v>2032</v>
       </c>
       <c r="H26" s="12">
-        <f>B26*(About!$A$16)/10^6</f>
-        <v>2.0135004E-5</v>
+        <f>B26*(About!$A$17)/10^6</f>
+        <v>1.8853000000000001E-5</v>
       </c>
       <c r="I26" s="12">
-        <f>C26*(About!$A$16)/10^6</f>
-        <v>6.1589423999999996E-5</v>
+        <f>C26*(About!$A$17)/10^6</f>
+        <v>5.7667999999999997E-5</v>
       </c>
       <c r="J26" s="12">
-        <f>D26*(About!$A$16)/10^6</f>
-        <v>8.8830899999999997E-5</v>
+        <f>D26*(About!$A$17)/10^6</f>
+        <v>8.3175000000000002E-5</v>
       </c>
       <c r="K26" s="12">
-        <f>E26*(About!$A$16)/10^6</f>
-        <v>1.87137096E-4</v>
-      </c>
-    </row>
-    <row r="27" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+        <f>E26*(About!$A$17)/10^6</f>
+        <v>1.75222E-4</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" s="13">
         <v>2033</v>
       </c>
@@ -1614,23 +1627,23 @@
         <v>2033</v>
       </c>
       <c r="H27" s="12">
-        <f>B27*(About!$A$16)/10^6</f>
-        <v>2.0135004E-5</v>
+        <f>B27*(About!$A$17)/10^6</f>
+        <v>1.8853000000000001E-5</v>
       </c>
       <c r="I27" s="12">
-        <f>C27*(About!$A$16)/10^6</f>
-        <v>6.2773835999999997E-5</v>
+        <f>C27*(About!$A$17)/10^6</f>
+        <v>5.8777000000000003E-5</v>
       </c>
       <c r="J27" s="12">
-        <f>D27*(About!$A$16)/10^6</f>
-        <v>9.0015311999999998E-5</v>
+        <f>D27*(About!$A$17)/10^6</f>
+        <v>8.4283999999999995E-5</v>
       </c>
       <c r="K27" s="12">
-        <f>E27*(About!$A$16)/10^6</f>
-        <v>1.9069033200000001E-4</v>
-      </c>
-    </row>
-    <row r="28" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+        <f>E27*(About!$A$17)/10^6</f>
+        <v>1.7854900000000001E-4</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" s="13">
         <v>2034</v>
       </c>
@@ -1651,23 +1664,23 @@
         <v>2034</v>
       </c>
       <c r="H28" s="12">
-        <f>B28*(About!$A$16)/10^6</f>
-        <v>2.1319416000000002E-5</v>
+        <f>B28*(About!$A$17)/10^6</f>
+        <v>1.9962E-5</v>
       </c>
       <c r="I28" s="12">
-        <f>C28*(About!$A$16)/10^6</f>
-        <v>6.3958247999999998E-5</v>
+        <f>C28*(About!$A$17)/10^6</f>
+        <v>5.9885999999999995E-5</v>
       </c>
       <c r="J28" s="12">
-        <f>D28*(About!$A$16)/10^6</f>
-        <v>9.1199723999999999E-5</v>
+        <f>D28*(About!$A$17)/10^6</f>
+        <v>8.5393E-5</v>
       </c>
       <c r="K28" s="12">
-        <f>E28*(About!$A$16)/10^6</f>
-        <v>1.9424356800000001E-4</v>
-      </c>
-    </row>
-    <row r="29" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+        <f>E28*(About!$A$17)/10^6</f>
+        <v>1.81876E-4</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" s="13">
         <v>2035</v>
       </c>
@@ -1688,23 +1701,23 @@
         <v>2035</v>
       </c>
       <c r="H29" s="12">
-        <f>B29*(About!$A$16)/10^6</f>
-        <v>2.1319416000000002E-5</v>
+        <f>B29*(About!$A$17)/10^6</f>
+        <v>1.9962E-5</v>
       </c>
       <c r="I29" s="12">
-        <f>C29*(About!$A$16)/10^6</f>
-        <v>6.5142660000000013E-5</v>
+        <f>C29*(About!$A$17)/10^6</f>
+        <v>6.0994999999999995E-5</v>
       </c>
       <c r="J29" s="12">
-        <f>D29*(About!$A$16)/10^6</f>
-        <v>9.2384136E-5</v>
+        <f>D29*(About!$A$17)/10^6</f>
+        <v>8.6501999999999993E-5</v>
       </c>
       <c r="K29" s="12">
-        <f>E29*(About!$A$16)/10^6</f>
-        <v>1.9898121600000002E-4</v>
-      </c>
-    </row>
-    <row r="30" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+        <f>E29*(About!$A$17)/10^6</f>
+        <v>1.86312E-4</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" s="13">
         <v>2036</v>
       </c>
@@ -1725,23 +1738,23 @@
         <v>2036</v>
       </c>
       <c r="H30" s="12">
-        <f>B30*(About!$A$16)/10^6</f>
-        <v>2.2503828E-5</v>
+        <f>B30*(About!$A$17)/10^6</f>
+        <v>2.1070999999999999E-5</v>
       </c>
       <c r="I30" s="12">
-        <f>C30*(About!$A$16)/10^6</f>
-        <v>6.6327072000000001E-5</v>
+        <f>C30*(About!$A$17)/10^6</f>
+        <v>6.2104E-5</v>
       </c>
       <c r="J30" s="12">
-        <f>D30*(About!$A$16)/10^6</f>
-        <v>9.3568548000000002E-5</v>
+        <f>D30*(About!$A$17)/10^6</f>
+        <v>8.7610999999999999E-5</v>
       </c>
       <c r="K30" s="12">
-        <f>E30*(About!$A$16)/10^6</f>
-        <v>2.0253445200000002E-4</v>
-      </c>
-    </row>
-    <row r="31" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+        <f>E30*(About!$A$17)/10^6</f>
+        <v>1.8963900000000002E-4</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" s="13">
         <v>2037</v>
       </c>
@@ -1762,23 +1775,23 @@
         <v>2037</v>
       </c>
       <c r="H31" s="12">
-        <f>B31*(About!$A$16)/10^6</f>
-        <v>2.2503828E-5</v>
+        <f>B31*(About!$A$17)/10^6</f>
+        <v>2.1070999999999999E-5</v>
       </c>
       <c r="I31" s="12">
-        <f>C31*(About!$A$16)/10^6</f>
-        <v>6.7511484000000002E-5</v>
+        <f>C31*(About!$A$17)/10^6</f>
+        <v>6.3213000000000006E-5</v>
       </c>
       <c r="J31" s="12">
-        <f>D31*(About!$A$16)/10^6</f>
-        <v>9.5937371999999991E-5</v>
+        <f>D31*(About!$A$17)/10^6</f>
+        <v>8.9828999999999997E-5</v>
       </c>
       <c r="K31" s="12">
-        <f>E31*(About!$A$16)/10^6</f>
-        <v>2.0608768800000002E-4</v>
-      </c>
-    </row>
-    <row r="32" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+        <f>E31*(About!$A$17)/10^6</f>
+        <v>1.9296600000000001E-4</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" s="13">
         <v>2038</v>
       </c>
@@ -1799,23 +1812,23 @@
         <v>2038</v>
       </c>
       <c r="H32" s="12">
-        <f>B32*(About!$A$16)/10^6</f>
-        <v>2.3688240000000001E-5</v>
+        <f>B32*(About!$A$17)/10^6</f>
+        <v>2.2180000000000001E-5</v>
       </c>
       <c r="I32" s="12">
-        <f>C32*(About!$A$16)/10^6</f>
-        <v>6.8695896000000003E-5</v>
+        <f>C32*(About!$A$17)/10^6</f>
+        <v>6.4321999999999998E-5</v>
       </c>
       <c r="J32" s="12">
-        <f>D32*(About!$A$16)/10^6</f>
-        <v>9.7121784000000005E-5</v>
+        <f>D32*(About!$A$17)/10^6</f>
+        <v>9.0938000000000002E-5</v>
       </c>
       <c r="K32" s="12">
-        <f>E32*(About!$A$16)/10^6</f>
-        <v>2.09640924E-4</v>
-      </c>
-    </row>
-    <row r="33" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+        <f>E32*(About!$A$17)/10^6</f>
+        <v>1.96293E-4</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33" s="13">
         <v>2039</v>
       </c>
@@ -1836,23 +1849,23 @@
         <v>2039</v>
       </c>
       <c r="H33" s="12">
-        <f>B33*(About!$A$16)/10^6</f>
-        <v>2.3688240000000001E-5</v>
+        <f>B33*(About!$A$17)/10^6</f>
+        <v>2.2180000000000001E-5</v>
       </c>
       <c r="I33" s="12">
-        <f>C33*(About!$A$16)/10^6</f>
-        <v>6.9880308000000004E-5</v>
+        <f>C33*(About!$A$17)/10^6</f>
+        <v>6.5430999999999991E-5</v>
       </c>
       <c r="J33" s="12">
-        <f>D33*(About!$A$16)/10^6</f>
-        <v>9.8306196000000007E-5</v>
+        <f>D33*(About!$A$17)/10^6</f>
+        <v>9.2046999999999995E-5</v>
       </c>
       <c r="K33" s="12">
-        <f>E33*(About!$A$16)/10^6</f>
-        <v>2.1319416E-4</v>
-      </c>
-    </row>
-    <row r="34" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+        <f>E33*(About!$A$17)/10^6</f>
+        <v>1.9962000000000002E-4</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34" s="13">
         <v>2040</v>
       </c>
@@ -1873,23 +1886,23 @@
         <v>2040</v>
       </c>
       <c r="H34" s="12">
-        <f>B34*(About!$A$16)/10^6</f>
-        <v>2.4872652000000002E-5</v>
+        <f>B34*(About!$A$17)/10^6</f>
+        <v>2.3289E-5</v>
       </c>
       <c r="I34" s="12">
-        <f>C34*(About!$A$16)/10^6</f>
-        <v>7.1064719999999992E-5</v>
+        <f>C34*(About!$A$17)/10^6</f>
+        <v>6.6539999999999997E-5</v>
       </c>
       <c r="J34" s="12">
-        <f>D34*(About!$A$16)/10^6</f>
-        <v>9.9490608000000008E-5</v>
+        <f>D34*(About!$A$17)/10^6</f>
+        <v>9.3156000000000001E-5</v>
       </c>
       <c r="K34" s="12">
-        <f>E34*(About!$A$16)/10^6</f>
-        <v>2.1674739600000001E-4</v>
-      </c>
-    </row>
-    <row r="35" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+        <f>E34*(About!$A$17)/10^6</f>
+        <v>2.0294700000000001E-4</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35" s="13">
         <v>2041</v>
       </c>
@@ -1910,23 +1923,23 @@
         <v>2041</v>
       </c>
       <c r="H35" s="12">
-        <f>B35*(About!$A$16)/10^6</f>
-        <v>2.4872652000000002E-5</v>
+        <f>B35*(About!$A$17)/10^6</f>
+        <v>2.3289E-5</v>
       </c>
       <c r="I35" s="12">
-        <f>C35*(About!$A$16)/10^6</f>
-        <v>7.2249132000000007E-5</v>
+        <f>C35*(About!$A$17)/10^6</f>
+        <v>6.7649000000000002E-5</v>
       </c>
       <c r="J35" s="12">
-        <f>D35*(About!$A$16)/10^6</f>
-        <v>1.0067502000000001E-4</v>
+        <f>D35*(About!$A$17)/10^6</f>
+        <v>9.4265000000000006E-5</v>
       </c>
       <c r="K35" s="12">
-        <f>E35*(About!$A$16)/10^6</f>
-        <v>2.2030063200000001E-4</v>
-      </c>
-    </row>
-    <row r="36" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+        <f>E35*(About!$A$17)/10^6</f>
+        <v>2.06274E-4</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36" s="13">
         <v>2042</v>
       </c>
@@ -1947,23 +1960,23 @@
         <v>2042</v>
       </c>
       <c r="H36" s="12">
-        <f>B36*(About!$A$16)/10^6</f>
-        <v>2.6057064E-5</v>
+        <f>B36*(About!$A$17)/10^6</f>
+        <v>2.4397999999999999E-5</v>
       </c>
       <c r="I36" s="12">
-        <f>C36*(About!$A$16)/10^6</f>
-        <v>7.2249132000000007E-5</v>
+        <f>C36*(About!$A$17)/10^6</f>
+        <v>6.7649000000000002E-5</v>
       </c>
       <c r="J36" s="12">
-        <f>D36*(About!$A$16)/10^6</f>
-        <v>1.01859432E-4</v>
+        <f>D36*(About!$A$17)/10^6</f>
+        <v>9.5373999999999999E-5</v>
       </c>
       <c r="K36" s="12">
-        <f>E36*(About!$A$16)/10^6</f>
-        <v>2.2385386800000001E-4</v>
-      </c>
-    </row>
-    <row r="37" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+        <f>E36*(About!$A$17)/10^6</f>
+        <v>2.0960099999999999E-4</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37" s="13">
         <v>2043</v>
       </c>
@@ -1984,23 +1997,23 @@
         <v>2043</v>
       </c>
       <c r="H37" s="12">
-        <f>B37*(About!$A$16)/10^6</f>
-        <v>2.6057064E-5</v>
+        <f>B37*(About!$A$17)/10^6</f>
+        <v>2.4397999999999999E-5</v>
       </c>
       <c r="I37" s="12">
-        <f>C37*(About!$A$16)/10^6</f>
-        <v>7.3433543999999994E-5</v>
+        <f>C37*(About!$A$17)/10^6</f>
+        <v>6.8757999999999995E-5</v>
       </c>
       <c r="J37" s="12">
-        <f>D37*(About!$A$16)/10^6</f>
-        <v>1.0304384400000001E-4</v>
+        <f>D37*(About!$A$17)/10^6</f>
+        <v>9.6483000000000004E-5</v>
       </c>
       <c r="K37" s="12">
-        <f>E37*(About!$A$16)/10^6</f>
-        <v>2.2740710399999999E-4</v>
-      </c>
-    </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.35">
+        <f>E37*(About!$A$17)/10^6</f>
+        <v>2.1292800000000001E-4</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38" s="13">
         <v>2044</v>
       </c>
@@ -2021,23 +2034,23 @@
         <v>2044</v>
       </c>
       <c r="H38" s="12">
-        <f>B38*(About!$A$16)/10^6</f>
-        <v>2.7241475999999998E-5</v>
+        <f>B38*(About!$A$17)/10^6</f>
+        <v>2.5506999999999998E-5</v>
       </c>
       <c r="I38" s="12">
-        <f>C38*(About!$A$16)/10^6</f>
-        <v>7.4617956000000009E-5</v>
+        <f>C38*(About!$A$17)/10^6</f>
+        <v>6.9867E-5</v>
       </c>
       <c r="J38" s="12">
-        <f>D38*(About!$A$16)/10^6</f>
-        <v>1.04228256E-4</v>
+        <f>D38*(About!$A$17)/10^6</f>
+        <v>9.7591999999999997E-5</v>
       </c>
       <c r="K38" s="12">
-        <f>E38*(About!$A$16)/10^6</f>
-        <v>2.2977592799999999E-4</v>
-      </c>
-    </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.35">
+        <f>E38*(About!$A$17)/10^6</f>
+        <v>2.1514599999999999E-4</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39" s="13">
         <v>2045</v>
       </c>
@@ -2058,23 +2071,23 @@
         <v>2045</v>
       </c>
       <c r="H39" s="12">
-        <f>B39*(About!$A$16)/10^6</f>
-        <v>2.7241475999999998E-5</v>
+        <f>B39*(About!$A$17)/10^6</f>
+        <v>2.5506999999999998E-5</v>
       </c>
       <c r="I39" s="12">
-        <f>C39*(About!$A$16)/10^6</f>
-        <v>7.5802367999999997E-5</v>
+        <f>C39*(About!$A$17)/10^6</f>
+        <v>7.0975999999999993E-5</v>
       </c>
       <c r="J39" s="12">
-        <f>D39*(About!$A$16)/10^6</f>
-        <v>1.05412668E-4</v>
+        <f>D39*(About!$A$17)/10^6</f>
+        <v>9.8700999999999989E-5</v>
       </c>
       <c r="K39" s="12">
-        <f>E39*(About!$A$16)/10^6</f>
-        <v>2.33329164E-4</v>
-      </c>
-    </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.35">
+        <f>E39*(About!$A$17)/10^6</f>
+        <v>2.1847299999999998E-4</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A40" s="13">
         <v>2046</v>
       </c>
@@ -2095,23 +2108,23 @@
         <v>2046</v>
       </c>
       <c r="H40" s="12">
-        <f>B40*(About!$A$16)/10^6</f>
-        <v>2.8425887999999999E-5</v>
+        <f>B40*(About!$A$17)/10^6</f>
+        <v>2.6616000000000001E-5</v>
       </c>
       <c r="I40" s="12">
-        <f>C40*(About!$A$16)/10^6</f>
-        <v>7.6986779999999998E-5</v>
+        <f>C40*(About!$A$17)/10^6</f>
+        <v>7.2084999999999998E-5</v>
       </c>
       <c r="J40" s="12">
-        <f>D40*(About!$A$16)/10^6</f>
-        <v>1.0659708E-4</v>
+        <f>D40*(About!$A$17)/10^6</f>
+        <v>9.9810000000000008E-5</v>
       </c>
       <c r="K40" s="12">
-        <f>E40*(About!$A$16)/10^6</f>
-        <v>2.3688240000000003E-4</v>
-      </c>
-    </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.35">
+        <f>E40*(About!$A$17)/10^6</f>
+        <v>2.2180000000000002E-4</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A41" s="13">
         <v>2047</v>
       </c>
@@ -2132,23 +2145,23 @@
         <v>2047</v>
       </c>
       <c r="H41" s="12">
-        <f>B41*(About!$A$16)/10^6</f>
-        <v>2.8425887999999999E-5</v>
+        <f>B41*(About!$A$17)/10^6</f>
+        <v>2.6616000000000001E-5</v>
       </c>
       <c r="I41" s="12">
-        <f>C41*(About!$A$16)/10^6</f>
-        <v>7.8171191999999999E-5</v>
+        <f>C41*(About!$A$17)/10^6</f>
+        <v>7.3194000000000004E-5</v>
       </c>
       <c r="J41" s="12">
-        <f>D41*(About!$A$16)/10^6</f>
-        <v>1.0896590399999999E-4</v>
+        <f>D41*(About!$A$17)/10^6</f>
+        <v>1.0202799999999999E-4</v>
       </c>
       <c r="K41" s="12">
-        <f>E41*(About!$A$16)/10^6</f>
-        <v>2.40435636E-4</v>
-      </c>
-    </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.35">
+        <f>E41*(About!$A$17)/10^6</f>
+        <v>2.2512700000000001E-4</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A42" s="13">
         <v>2048</v>
       </c>
@@ -2169,23 +2182,23 @@
         <v>2048</v>
       </c>
       <c r="H42" s="12">
-        <f>B42*(About!$A$16)/10^6</f>
-        <v>2.9610300000000003E-5</v>
+        <f>B42*(About!$A$17)/10^6</f>
+        <v>2.7725000000000003E-5</v>
       </c>
       <c r="I42" s="12">
-        <f>C42*(About!$A$16)/10^6</f>
-        <v>7.9355604000000001E-5</v>
+        <f>C42*(About!$A$17)/10^6</f>
+        <v>7.4302999999999997E-5</v>
       </c>
       <c r="J42" s="12">
-        <f>D42*(About!$A$16)/10^6</f>
-        <v>1.1015031600000001E-4</v>
+        <f>D42*(About!$A$17)/10^6</f>
+        <v>1.03137E-4</v>
       </c>
       <c r="K42" s="12">
-        <f>E42*(About!$A$16)/10^6</f>
-        <v>2.4398887200000001E-4</v>
-      </c>
-    </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.35">
+        <f>E42*(About!$A$17)/10^6</f>
+        <v>2.2845400000000001E-4</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A43" s="13">
         <v>2049</v>
       </c>
@@ -2206,23 +2219,23 @@
         <v>2049</v>
       </c>
       <c r="H43" s="12">
-        <f>B43*(About!$A$16)/10^6</f>
-        <v>2.9610300000000003E-5</v>
+        <f>B43*(About!$A$17)/10^6</f>
+        <v>2.7725000000000003E-5</v>
       </c>
       <c r="I43" s="12">
-        <f>C43*(About!$A$16)/10^6</f>
-        <v>8.0540016000000002E-5</v>
+        <f>C43*(About!$A$17)/10^6</f>
+        <v>7.5412000000000002E-5</v>
       </c>
       <c r="J43" s="12">
-        <f>D43*(About!$A$16)/10^6</f>
-        <v>1.1133472799999999E-4</v>
+        <f>D43*(About!$A$17)/10^6</f>
+        <v>1.0424599999999999E-4</v>
       </c>
       <c r="K43" s="12">
-        <f>E43*(About!$A$16)/10^6</f>
-        <v>2.4754210800000001E-4</v>
-      </c>
-    </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.35">
+        <f>E43*(About!$A$17)/10^6</f>
+        <v>2.31781E-4</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A44" s="13">
         <v>2050</v>
       </c>
@@ -2243,20 +2256,20 @@
         <v>2050</v>
       </c>
       <c r="H44" s="12">
-        <f>B44*(About!$A$16)/10^6</f>
-        <v>3.0794711999999998E-5</v>
+        <f>B44*(About!$A$17)/10^6</f>
+        <v>2.8833999999999999E-5</v>
       </c>
       <c r="I44" s="12">
-        <f>C44*(About!$A$16)/10^6</f>
-        <v>8.1724428000000003E-5</v>
+        <f>C44*(About!$A$17)/10^6</f>
+        <v>7.6520999999999995E-5</v>
       </c>
       <c r="J44" s="12">
-        <f>D44*(About!$A$16)/10^6</f>
-        <v>1.1251914000000001E-4</v>
+        <f>D44*(About!$A$17)/10^6</f>
+        <v>1.0535500000000001E-4</v>
       </c>
       <c r="K44" s="12">
-        <f>E44*(About!$A$16)/10^6</f>
-        <v>2.5109534399999999E-4</v>
+        <f>E44*(About!$A$17)/10^6</f>
+        <v>2.3510800000000001E-4</v>
       </c>
     </row>
   </sheetData>
@@ -2272,430 +2285,430 @@
   <dimension ref="A1:B42"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="24.1796875" customWidth="1"/>
+    <col min="2" max="2" width="24.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>4</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2">
         <f>SourceData!G4</f>
         <v>2010</v>
       </c>
       <c r="B2" s="12">
         <f>SourceData!I4</f>
-        <v>3.6716771999999997E-5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+        <v>3.4378999999999997E-5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3">
         <f>SourceData!G5</f>
         <v>2011</v>
       </c>
       <c r="B3" s="12">
         <f>SourceData!I5</f>
-        <v>3.7901183999999998E-5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+        <v>3.5487999999999996E-5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4">
         <f>SourceData!G6</f>
         <v>2012</v>
       </c>
       <c r="B4" s="12">
         <f>SourceData!I6</f>
-        <v>3.9085596E-5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+        <v>3.6597000000000002E-5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5">
         <f>SourceData!G7</f>
         <v>2013</v>
       </c>
       <c r="B5" s="12">
         <f>SourceData!I7</f>
-        <v>4.0270008000000001E-5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+        <v>3.7706000000000001E-5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6">
         <f>SourceData!G8</f>
         <v>2014</v>
       </c>
       <c r="B6" s="12">
         <f>SourceData!I8</f>
-        <v>4.1454420000000002E-5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+        <v>3.8815E-5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7">
         <f>SourceData!G9</f>
         <v>2015</v>
       </c>
       <c r="B7" s="12">
         <f>SourceData!I9</f>
-        <v>4.2638832000000003E-5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+        <v>3.9923999999999999E-5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8">
         <f>SourceData!G10</f>
         <v>2016</v>
       </c>
       <c r="B8" s="12">
         <f>SourceData!I10</f>
-        <v>4.5007655999999999E-5</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+        <v>4.2141999999999997E-5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9">
         <f>SourceData!G11</f>
         <v>2017</v>
       </c>
       <c r="B9" s="12">
         <f>SourceData!I11</f>
-        <v>4.6192068E-5</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+        <v>4.3250999999999996E-5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10">
         <f>SourceData!G12</f>
         <v>2018</v>
       </c>
       <c r="B10" s="12">
         <f>SourceData!I12</f>
-        <v>4.7376480000000001E-5</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+        <v>4.4360000000000002E-5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11">
         <f>SourceData!G13</f>
         <v>2019</v>
       </c>
       <c r="B11" s="12">
         <f>SourceData!I13</f>
-        <v>4.8560892000000003E-5</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+        <v>4.5469000000000001E-5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12">
         <f>SourceData!G14</f>
         <v>2020</v>
       </c>
       <c r="B12" s="12">
         <f>SourceData!I14</f>
-        <v>4.9745304000000004E-5</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+        <v>4.6578E-5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13">
         <f>SourceData!G15</f>
         <v>2021</v>
       </c>
       <c r="B13" s="12">
         <f>SourceData!I15</f>
-        <v>4.9745304000000004E-5</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+        <v>4.6578E-5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14">
         <f>SourceData!G16</f>
         <v>2022</v>
       </c>
       <c r="B14" s="12">
         <f>SourceData!I16</f>
-        <v>5.0929715999999998E-5</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+        <v>4.7686999999999999E-5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15">
         <f>SourceData!G17</f>
         <v>2023</v>
       </c>
       <c r="B15" s="12">
         <f>SourceData!I17</f>
-        <v>5.2114128E-5</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+        <v>4.8795999999999998E-5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16">
         <f>SourceData!G18</f>
         <v>2024</v>
       </c>
       <c r="B16" s="12">
         <f>SourceData!I18</f>
-        <v>5.3298540000000001E-5</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+        <v>4.9905000000000004E-5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17">
         <f>SourceData!G19</f>
         <v>2025</v>
       </c>
       <c r="B17" s="12">
         <f>SourceData!I19</f>
-        <v>5.4482951999999995E-5</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+        <v>5.1013999999999996E-5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18">
         <f>SourceData!G20</f>
         <v>2026</v>
       </c>
       <c r="B18" s="12">
         <f>SourceData!I20</f>
-        <v>5.5667363999999996E-5</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+        <v>5.2122999999999995E-5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19">
         <f>SourceData!G21</f>
         <v>2027</v>
       </c>
       <c r="B19" s="12">
         <f>SourceData!I21</f>
-        <v>5.6851775999999998E-5</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+        <v>5.3232000000000001E-5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20">
         <f>SourceData!G22</f>
         <v>2028</v>
       </c>
       <c r="B20" s="12">
         <f>SourceData!I22</f>
-        <v>5.8036188000000006E-5</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+        <v>5.4341E-5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21">
         <f>SourceData!G23</f>
         <v>2029</v>
       </c>
       <c r="B21" s="12">
         <f>SourceData!I23</f>
-        <v>5.8036188000000006E-5</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+        <v>5.4341E-5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22">
         <f>SourceData!G24</f>
         <v>2030</v>
       </c>
       <c r="B22" s="12">
         <f>SourceData!I24</f>
-        <v>5.9220600000000007E-5</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+        <v>5.5450000000000006E-5</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23">
         <f>SourceData!G25</f>
         <v>2031</v>
       </c>
       <c r="B23" s="12">
         <f>SourceData!I25</f>
-        <v>6.0405012000000001E-5</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+        <v>5.6558999999999998E-5</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24">
         <f>SourceData!G26</f>
         <v>2032</v>
       </c>
       <c r="B24" s="12">
         <f>SourceData!I26</f>
-        <v>6.1589423999999996E-5</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+        <v>5.7667999999999997E-5</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25">
         <f>SourceData!G27</f>
         <v>2033</v>
       </c>
       <c r="B25" s="12">
         <f>SourceData!I27</f>
-        <v>6.2773835999999997E-5</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+        <v>5.8777000000000003E-5</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26">
         <f>SourceData!G28</f>
         <v>2034</v>
       </c>
       <c r="B26" s="12">
         <f>SourceData!I28</f>
-        <v>6.3958247999999998E-5</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+        <v>5.9885999999999995E-5</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27">
         <f>SourceData!G29</f>
         <v>2035</v>
       </c>
       <c r="B27" s="12">
         <f>SourceData!I29</f>
-        <v>6.5142660000000013E-5</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+        <v>6.0994999999999995E-5</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28">
         <f>SourceData!G30</f>
         <v>2036</v>
       </c>
       <c r="B28" s="12">
         <f>SourceData!I30</f>
-        <v>6.6327072000000001E-5</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+        <v>6.2104E-5</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29">
         <f>SourceData!G31</f>
         <v>2037</v>
       </c>
       <c r="B29" s="12">
         <f>SourceData!I31</f>
-        <v>6.7511484000000002E-5</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+        <v>6.3213000000000006E-5</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30">
         <f>SourceData!G32</f>
         <v>2038</v>
       </c>
       <c r="B30" s="12">
         <f>SourceData!I32</f>
-        <v>6.8695896000000003E-5</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+        <v>6.4321999999999998E-5</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31">
         <f>SourceData!G33</f>
         <v>2039</v>
       </c>
       <c r="B31" s="12">
         <f>SourceData!I33</f>
-        <v>6.9880308000000004E-5</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+        <v>6.5430999999999991E-5</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32">
         <f>SourceData!G34</f>
         <v>2040</v>
       </c>
       <c r="B32" s="12">
         <f>SourceData!I34</f>
-        <v>7.1064719999999992E-5</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+        <v>6.6539999999999997E-5</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33">
         <f>SourceData!G35</f>
         <v>2041</v>
       </c>
       <c r="B33" s="12">
         <f>SourceData!I35</f>
-        <v>7.2249132000000007E-5</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+        <v>6.7649000000000002E-5</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34">
         <f>SourceData!G36</f>
         <v>2042</v>
       </c>
       <c r="B34" s="12">
         <f>SourceData!I36</f>
-        <v>7.2249132000000007E-5</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+        <v>6.7649000000000002E-5</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35">
         <f>SourceData!G37</f>
         <v>2043</v>
       </c>
       <c r="B35" s="12">
         <f>SourceData!I37</f>
-        <v>7.3433543999999994E-5</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+        <v>6.8757999999999995E-5</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36">
         <f>SourceData!G38</f>
         <v>2044</v>
       </c>
       <c r="B36" s="12">
         <f>SourceData!I38</f>
-        <v>7.4617956000000009E-5</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.35">
+        <v>6.9867E-5</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37">
         <f>SourceData!G39</f>
         <v>2045</v>
       </c>
       <c r="B37" s="12">
         <f>SourceData!I39</f>
-        <v>7.5802367999999997E-5</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.35">
+        <v>7.0975999999999993E-5</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38">
         <f>SourceData!G40</f>
         <v>2046</v>
       </c>
       <c r="B38" s="12">
         <f>SourceData!I40</f>
-        <v>7.6986779999999998E-5</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.35">
+        <v>7.2084999999999998E-5</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A39">
         <f>SourceData!G41</f>
         <v>2047</v>
       </c>
       <c r="B39" s="12">
         <f>SourceData!I41</f>
-        <v>7.8171191999999999E-5</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.35">
+        <v>7.3194000000000004E-5</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A40">
         <f>SourceData!G42</f>
         <v>2048</v>
       </c>
       <c r="B40" s="12">
         <f>SourceData!I42</f>
-        <v>7.9355604000000001E-5</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.35">
+        <v>7.4302999999999997E-5</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A41">
         <f>SourceData!G43</f>
         <v>2049</v>
       </c>
       <c r="B41" s="12">
         <f>SourceData!I43</f>
-        <v>8.0540016000000002E-5</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.35">
+        <v>7.5412000000000002E-5</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42">
         <f>SourceData!G44</f>
         <v>2050</v>
       </c>
       <c r="B42" s="12">
         <f>SourceData!I44</f>
-        <v>8.1724428000000003E-5</v>
+        <v>7.6520999999999995E-5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updates to RMI data
</commit_message>
<xml_diff>
--- a/InputData/add-outputs/SCoC/Social Cost of Carbon.xlsx
+++ b/InputData/add-outputs/SCoC/Social Cost of Carbon.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10411"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24527"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/users/nathaniyer/library/containers/com.microsoft.excel/data/state-eps-data-repository/template_state/add-outputs/scoc/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\olivia\Documents\EPS_Models by Region\RMI\All_states_RMI\CA\add-outputs\SCoC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DDF0DC7-9A6E-564A-84AD-DEF2A1FA8985}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{C7DFA844-B094-464D-A0ED-5509A31E1148}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="460" windowWidth="21080" windowHeight="11820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1150" yWindow="570" windowWidth="16460" windowHeight="13230" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="23">
   <si>
     <t>Source:</t>
   </si>
@@ -99,6 +99,9 @@
   </si>
   <si>
     <t>ton of carbon dioxide emitted, the U.S. government typically uses the figures based on</t>
+  </si>
+  <si>
+    <t>California</t>
   </si>
 </sst>
 </file>
@@ -621,20 +624,23 @@
       <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="97.1640625" customWidth="1"/>
+    <col min="2" max="2" width="97.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="B1" t="s">
+        <v>22</v>
+      </c>
       <c r="C1" s="14">
-        <v>44307</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+        <v>44509</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
@@ -642,67 +648,67 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B4" s="2">
         <v>2015</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B5" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B6" s="3" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B7" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="11" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A11" s="13" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A16" s="13" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A17" s="13">
         <v>1.109</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A18" s="13" t="s">
         <v>15</v>
       </c>
@@ -719,13 +725,13 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="13.5" customWidth="1"/>
-    <col min="7" max="7" width="13.83203125" customWidth="1"/>
+    <col min="1" max="1" width="13.453125" customWidth="1"/>
+    <col min="7" max="7" width="13.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A1" s="8" t="s">
         <v>8</v>
       </c>
@@ -741,7 +747,7 @@
       <c r="J1" s="11"/>
       <c r="K1" s="11"/>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A2" s="5" t="s">
         <v>3</v>
       </c>
@@ -773,7 +779,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A3" s="5" t="s">
         <v>5</v>
       </c>
@@ -805,7 +811,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A4" s="13">
         <v>2010</v>
       </c>
@@ -842,7 +848,7 @@
         <v>9.5373999999999999E-5</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A5" s="13">
         <v>2011</v>
       </c>
@@ -879,7 +885,7 @@
         <v>9.9810000000000008E-5</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A6" s="13">
         <v>2012</v>
       </c>
@@ -916,7 +922,7 @@
         <v>1.03137E-4</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A7" s="13">
         <v>2013</v>
       </c>
@@ -953,7 +959,7 @@
         <v>1.0757299999999999E-4</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A8" s="13">
         <v>2014</v>
       </c>
@@ -990,7 +996,7 @@
         <v>1.12009E-4</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A9" s="13">
         <v>2015</v>
       </c>
@@ -1027,7 +1033,7 @@
         <v>1.1644499999999999E-4</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A10" s="13">
         <v>2016</v>
       </c>
@@ -1064,7 +1070,7 @@
         <v>1.1977199999999999E-4</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A11" s="13">
         <v>2017</v>
       </c>
@@ -1101,7 +1107,7 @@
         <v>1.24208E-4</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A12" s="13">
         <v>2018</v>
       </c>
@@ -1138,7 +1144,7 @@
         <v>1.28644E-4</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A13" s="13">
         <v>2019</v>
       </c>
@@ -1175,7 +1181,7 @@
         <v>1.3307999999999999E-4</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A14" s="13">
         <v>2020</v>
       </c>
@@ -1212,7 +1218,7 @@
         <v>1.3640700000000001E-4</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A15" s="13">
         <v>2021</v>
       </c>
@@ -1249,7 +1255,7 @@
         <v>1.39734E-4</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A16" s="13">
         <v>2022</v>
       </c>
@@ -1286,7 +1292,7 @@
         <v>1.4306100000000002E-4</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A17" s="13">
         <v>2023</v>
       </c>
@@ -1323,7 +1329,7 @@
         <v>1.4638800000000001E-4</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A18" s="13">
         <v>2024</v>
       </c>
@@ -1360,7 +1366,7 @@
         <v>1.49715E-4</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A19" s="13">
         <v>2025</v>
       </c>
@@ -1397,7 +1403,7 @@
         <v>1.5304199999999999E-4</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A20" s="13">
         <v>2026</v>
       </c>
@@ -1434,7 +1440,7 @@
         <v>1.5636900000000001E-4</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A21" s="13">
         <v>2027</v>
       </c>
@@ -1471,7 +1477,7 @@
         <v>1.5858699999999999E-4</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A22" s="13">
         <v>2028</v>
       </c>
@@ -1508,7 +1514,7 @@
         <v>1.6191399999999998E-4</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A23" s="13">
         <v>2029</v>
       </c>
@@ -1545,7 +1551,7 @@
         <v>1.65241E-4</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A24" s="13">
         <v>2030</v>
       </c>
@@ -1582,7 +1588,7 @@
         <v>1.6856799999999999E-4</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A25" s="13">
         <v>2031</v>
       </c>
@@ -1619,7 +1625,7 @@
         <v>1.7189500000000001E-4</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A26" s="13">
         <v>2032</v>
       </c>
@@ -1656,7 +1662,7 @@
         <v>1.75222E-4</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A27" s="13">
         <v>2033</v>
       </c>
@@ -1693,7 +1699,7 @@
         <v>1.7854900000000001E-4</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A28" s="13">
         <v>2034</v>
       </c>
@@ -1730,7 +1736,7 @@
         <v>1.81876E-4</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A29" s="13">
         <v>2035</v>
       </c>
@@ -1767,7 +1773,7 @@
         <v>1.86312E-4</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A30" s="13">
         <v>2036</v>
       </c>
@@ -1804,7 +1810,7 @@
         <v>1.8963900000000002E-4</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A31" s="13">
         <v>2037</v>
       </c>
@@ -1841,7 +1847,7 @@
         <v>1.9296600000000001E-4</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A32" s="13">
         <v>2038</v>
       </c>
@@ -1878,7 +1884,7 @@
         <v>1.96293E-4</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A33" s="13">
         <v>2039</v>
       </c>
@@ -1915,7 +1921,7 @@
         <v>1.9962000000000002E-4</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A34" s="13">
         <v>2040</v>
       </c>
@@ -1952,7 +1958,7 @@
         <v>2.0294700000000001E-4</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A35" s="13">
         <v>2041</v>
       </c>
@@ -1989,7 +1995,7 @@
         <v>2.06274E-4</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A36" s="13">
         <v>2042</v>
       </c>
@@ -2026,7 +2032,7 @@
         <v>2.0960099999999999E-4</v>
       </c>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A37" s="13">
         <v>2043</v>
       </c>
@@ -2063,7 +2069,7 @@
         <v>2.1292800000000001E-4</v>
       </c>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A38" s="13">
         <v>2044</v>
       </c>
@@ -2100,7 +2106,7 @@
         <v>2.1514599999999999E-4</v>
       </c>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A39" s="13">
         <v>2045</v>
       </c>
@@ -2137,7 +2143,7 @@
         <v>2.1847299999999998E-4</v>
       </c>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A40" s="13">
         <v>2046</v>
       </c>
@@ -2174,7 +2180,7 @@
         <v>2.2180000000000002E-4</v>
       </c>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A41" s="13">
         <v>2047</v>
       </c>
@@ -2211,7 +2217,7 @@
         <v>2.2512700000000001E-4</v>
       </c>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A42" s="13">
         <v>2048</v>
       </c>
@@ -2248,7 +2254,7 @@
         <v>2.2845400000000001E-4</v>
       </c>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A43" s="13">
         <v>2049</v>
       </c>
@@ -2285,7 +2291,7 @@
         <v>2.31781E-4</v>
       </c>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A44" s="13">
         <v>2050</v>
       </c>
@@ -2338,12 +2344,12 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="24.1640625" customWidth="1"/>
+    <col min="2" max="2" width="24.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="5" t="s">
         <v>4</v>
       </c>
@@ -2351,7 +2357,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2">
         <f>SourceData!G4</f>
         <v>2010</v>
@@ -2361,7 +2367,7 @@
         <v>3.4378999999999997E-5</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3">
         <f>SourceData!G5</f>
         <v>2011</v>
@@ -2371,7 +2377,7 @@
         <v>3.5487999999999996E-5</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4">
         <f>SourceData!G6</f>
         <v>2012</v>
@@ -2381,7 +2387,7 @@
         <v>3.6597000000000002E-5</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5">
         <f>SourceData!G7</f>
         <v>2013</v>
@@ -2391,7 +2397,7 @@
         <v>3.7706000000000001E-5</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6">
         <f>SourceData!G8</f>
         <v>2014</v>
@@ -2401,7 +2407,7 @@
         <v>3.8815E-5</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7">
         <f>SourceData!G9</f>
         <v>2015</v>
@@ -2411,7 +2417,7 @@
         <v>3.9923999999999999E-5</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8">
         <f>SourceData!G10</f>
         <v>2016</v>
@@ -2421,7 +2427,7 @@
         <v>4.2141999999999997E-5</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9">
         <f>SourceData!G11</f>
         <v>2017</v>
@@ -2431,7 +2437,7 @@
         <v>4.3250999999999996E-5</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10">
         <f>SourceData!G12</f>
         <v>2018</v>
@@ -2441,7 +2447,7 @@
         <v>4.4360000000000002E-5</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11">
         <f>SourceData!G13</f>
         <v>2019</v>
@@ -2451,7 +2457,7 @@
         <v>4.5469000000000001E-5</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12">
         <f>SourceData!G14</f>
         <v>2020</v>
@@ -2461,7 +2467,7 @@
         <v>4.6578E-5</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13">
         <f>SourceData!G15</f>
         <v>2021</v>
@@ -2471,7 +2477,7 @@
         <v>4.6578E-5</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14">
         <f>SourceData!G16</f>
         <v>2022</v>
@@ -2481,7 +2487,7 @@
         <v>4.7686999999999999E-5</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A15">
         <f>SourceData!G17</f>
         <v>2023</v>
@@ -2491,7 +2497,7 @@
         <v>4.8795999999999998E-5</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A16">
         <f>SourceData!G18</f>
         <v>2024</v>
@@ -2501,7 +2507,7 @@
         <v>4.9905000000000004E-5</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A17">
         <f>SourceData!G19</f>
         <v>2025</v>
@@ -2511,7 +2517,7 @@
         <v>5.1013999999999996E-5</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A18">
         <f>SourceData!G20</f>
         <v>2026</v>
@@ -2521,7 +2527,7 @@
         <v>5.2122999999999995E-5</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A19">
         <f>SourceData!G21</f>
         <v>2027</v>
@@ -2531,7 +2537,7 @@
         <v>5.3232000000000001E-5</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A20">
         <f>SourceData!G22</f>
         <v>2028</v>
@@ -2541,7 +2547,7 @@
         <v>5.4341E-5</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A21">
         <f>SourceData!G23</f>
         <v>2029</v>
@@ -2551,7 +2557,7 @@
         <v>5.4341E-5</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A22">
         <f>SourceData!G24</f>
         <v>2030</v>
@@ -2561,7 +2567,7 @@
         <v>5.5450000000000006E-5</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A23">
         <f>SourceData!G25</f>
         <v>2031</v>
@@ -2571,7 +2577,7 @@
         <v>5.6558999999999998E-5</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A24">
         <f>SourceData!G26</f>
         <v>2032</v>
@@ -2581,7 +2587,7 @@
         <v>5.7667999999999997E-5</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A25">
         <f>SourceData!G27</f>
         <v>2033</v>
@@ -2591,7 +2597,7 @@
         <v>5.8777000000000003E-5</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A26">
         <f>SourceData!G28</f>
         <v>2034</v>
@@ -2601,7 +2607,7 @@
         <v>5.9885999999999995E-5</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A27">
         <f>SourceData!G29</f>
         <v>2035</v>
@@ -2611,7 +2617,7 @@
         <v>6.0994999999999995E-5</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A28">
         <f>SourceData!G30</f>
         <v>2036</v>
@@ -2621,7 +2627,7 @@
         <v>6.2104E-5</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A29">
         <f>SourceData!G31</f>
         <v>2037</v>
@@ -2631,7 +2637,7 @@
         <v>6.3213000000000006E-5</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A30">
         <f>SourceData!G32</f>
         <v>2038</v>
@@ -2641,7 +2647,7 @@
         <v>6.4321999999999998E-5</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A31">
         <f>SourceData!G33</f>
         <v>2039</v>
@@ -2651,7 +2657,7 @@
         <v>6.5430999999999991E-5</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A32">
         <f>SourceData!G34</f>
         <v>2040</v>
@@ -2661,7 +2667,7 @@
         <v>6.6539999999999997E-5</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A33">
         <f>SourceData!G35</f>
         <v>2041</v>
@@ -2671,7 +2677,7 @@
         <v>6.7649000000000002E-5</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A34">
         <f>SourceData!G36</f>
         <v>2042</v>
@@ -2681,7 +2687,7 @@
         <v>6.7649000000000002E-5</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A35">
         <f>SourceData!G37</f>
         <v>2043</v>
@@ -2691,7 +2697,7 @@
         <v>6.8757999999999995E-5</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A36">
         <f>SourceData!G38</f>
         <v>2044</v>
@@ -2701,7 +2707,7 @@
         <v>6.9867E-5</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A37">
         <f>SourceData!G39</f>
         <v>2045</v>
@@ -2711,7 +2717,7 @@
         <v>7.0975999999999993E-5</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A38">
         <f>SourceData!G40</f>
         <v>2046</v>
@@ -2721,7 +2727,7 @@
         <v>7.2084999999999998E-5</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A39">
         <f>SourceData!G41</f>
         <v>2047</v>
@@ -2731,7 +2737,7 @@
         <v>7.3194000000000004E-5</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A40">
         <f>SourceData!G42</f>
         <v>2048</v>
@@ -2741,7 +2747,7 @@
         <v>7.4302999999999997E-5</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A41">
         <f>SourceData!G43</f>
         <v>2049</v>
@@ -2751,7 +2757,7 @@
         <v>7.5412000000000002E-5</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A42">
         <f>SourceData!G44</f>
         <v>2050</v>

</xml_diff>